<commit_message>
Ajout synthese des chiffres sur recuit
</commit_message>
<xml_diff>
--- a/tp2-A18/exemple/resultats/recuit_1.xlsx
+++ b/tp2-A18/exemple/resultats/recuit_1.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\inf4705_labs\tp2-A18\exemple\resultats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E182AFE-5691-465B-ACD0-619F9A9F1AD1}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A556349-EDB4-4239-A5DC-434DD68A29B0}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16428" windowHeight="8664"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="16428" windowHeight="8664" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="recuit_1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -106,7 +114,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -940,10 +948,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B297"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E298"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A270" workbookViewId="0">
+      <selection activeCell="D278" sqref="D278"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -1069,7 +1079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1.5622377E-2</v>
       </c>
@@ -1077,15 +1087,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>0</v>
       </c>
       <c r="B18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D18">
+        <f>AVERAGE(A13:A22)</f>
+        <v>1.8614769E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2.992392E-3</v>
       </c>
@@ -1093,7 +1107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>0</v>
       </c>
@@ -1101,7 +1115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>0</v>
       </c>
@@ -1109,7 +1123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>0</v>
       </c>
@@ -1117,20 +1131,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>0</v>
       </c>
       <c r="B24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D24">
+        <f>AVERAGE(A24:A33)</f>
+        <v>4.8861264999999999E-3</v>
+      </c>
+      <c r="E24">
+        <f>AVERAGE(B24:B33)</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>1.5622377E-2</v>
       </c>
@@ -1138,7 +1160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>1.5622139E-2</v>
       </c>
@@ -1146,7 +1168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>0</v>
       </c>
@@ -1154,7 +1176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>0</v>
       </c>
@@ -1162,7 +1184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>0</v>
       </c>
@@ -1170,7 +1192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>1.9941329999999999E-3</v>
       </c>
@@ -1178,7 +1200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>0</v>
       </c>
@@ -1186,7 +1208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>0</v>
       </c>
@@ -1194,7 +1216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>1.5622616000000001E-2</v>
       </c>
@@ -1202,20 +1224,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>1.99461E-3</v>
       </c>
       <c r="B35">
         <v>4</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D35">
+        <f t="shared" ref="D35:E35" si="0">AVERAGE(A35:A44)</f>
+        <v>6.037951E-4</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>0</v>
       </c>
@@ -1223,7 +1253,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>0</v>
       </c>
@@ -1231,7 +1261,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>0</v>
       </c>
@@ -1239,7 +1269,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>0</v>
       </c>
@@ -1247,7 +1277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>0</v>
       </c>
@@ -1255,7 +1285,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>2.0208359999999998E-3</v>
       </c>
@@ -1263,7 +1293,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>0</v>
       </c>
@@ -1271,7 +1301,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>0</v>
       </c>
@@ -1279,7 +1309,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>2.022505E-3</v>
       </c>
@@ -1287,20 +1317,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>0</v>
       </c>
       <c r="B46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D46">
+        <f t="shared" ref="D36:D99" si="1">AVERAGE(A46:A55)</f>
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <f t="shared" ref="E36:E99" si="2">AVERAGE(B46:B55)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>0</v>
       </c>
@@ -1308,7 +1346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>0</v>
       </c>
@@ -1316,7 +1354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>0</v>
       </c>
@@ -1324,7 +1362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>0</v>
       </c>
@@ -1332,7 +1370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>0</v>
       </c>
@@ -1340,7 +1378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>0</v>
       </c>
@@ -1348,7 +1386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>0</v>
       </c>
@@ -1356,7 +1394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>0</v>
       </c>
@@ -1364,7 +1402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>0</v>
       </c>
@@ -1372,20 +1410,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>9.9611300000000008E-4</v>
       </c>
       <c r="B57">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D57">
+        <f t="shared" si="1"/>
+        <v>1.7614364E-3</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="2"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>0</v>
       </c>
@@ -1393,7 +1439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>1.5620708000000001E-2</v>
       </c>
@@ -1401,7 +1447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>0</v>
       </c>
@@ -1409,7 +1455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>0</v>
       </c>
@@ -1417,7 +1463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>0</v>
       </c>
@@ -1425,7 +1471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>0</v>
       </c>
@@ -1433,7 +1479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>0</v>
       </c>
@@ -1441,7 +1487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>0</v>
       </c>
@@ -1449,7 +1495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>9.9754300000000004E-4</v>
       </c>
@@ -1457,20 +1503,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>0</v>
       </c>
       <c r="B68">
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D68">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E68">
+        <f t="shared" si="2"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>0</v>
       </c>
@@ -1478,7 +1532,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>0</v>
       </c>
@@ -1486,7 +1540,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>0</v>
       </c>
@@ -1494,7 +1548,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>0</v>
       </c>
@@ -1502,7 +1556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>0</v>
       </c>
@@ -1510,7 +1564,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>0</v>
       </c>
@@ -1518,7 +1572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>0</v>
       </c>
@@ -1526,7 +1580,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>0</v>
       </c>
@@ -1534,7 +1588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>0</v>
       </c>
@@ -1542,20 +1596,28 @@
         <v>8</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>0</v>
       </c>
       <c r="B79">
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D79">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E79">
+        <f t="shared" si="2"/>
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>0</v>
       </c>
@@ -1563,7 +1625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>0</v>
       </c>
@@ -1571,7 +1633,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>0</v>
       </c>
@@ -1579,7 +1641,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>0</v>
       </c>
@@ -1587,7 +1649,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>0</v>
       </c>
@@ -1595,7 +1657,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>0</v>
       </c>
@@ -1603,7 +1665,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>0</v>
       </c>
@@ -1611,7 +1673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>0</v>
       </c>
@@ -1619,7 +1681,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>0</v>
       </c>
@@ -1627,20 +1689,28 @@
         <v>7</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>0</v>
       </c>
       <c r="B90">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D90">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E90">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>0</v>
       </c>
@@ -1648,7 +1718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>0</v>
       </c>
@@ -1656,7 +1726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>0</v>
       </c>
@@ -1664,7 +1734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>0</v>
       </c>
@@ -1672,7 +1742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>0</v>
       </c>
@@ -1680,7 +1750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>0</v>
       </c>
@@ -1688,7 +1758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>0</v>
       </c>
@@ -1696,7 +1766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>0</v>
       </c>
@@ -1704,7 +1774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>0</v>
       </c>
@@ -1712,20 +1782,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>0</v>
       </c>
       <c r="B101">
         <v>1</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D101">
+        <f t="shared" ref="D100:D163" si="3">AVERAGE(A101:A110)</f>
+        <v>0</v>
+      </c>
+      <c r="E101">
+        <f t="shared" ref="E100:E163" si="4">AVERAGE(B101:B110)</f>
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>0</v>
       </c>
@@ -1733,7 +1811,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>0</v>
       </c>
@@ -1741,7 +1819,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>0</v>
       </c>
@@ -1749,7 +1827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>0</v>
       </c>
@@ -1757,7 +1835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>0</v>
       </c>
@@ -1765,7 +1843,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>0</v>
       </c>
@@ -1773,7 +1851,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>0</v>
       </c>
@@ -1781,7 +1859,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>0</v>
       </c>
@@ -1789,7 +1867,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>0</v>
       </c>
@@ -1797,20 +1875,28 @@
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>0</v>
       </c>
       <c r="B112">
         <v>95</v>
       </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D112">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E112">
+        <f t="shared" si="4"/>
+        <v>49.8</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>0</v>
       </c>
@@ -1818,7 +1904,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>0</v>
       </c>
@@ -1826,7 +1912,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>0</v>
       </c>
@@ -1834,7 +1920,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>0</v>
       </c>
@@ -1842,7 +1928,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>0</v>
       </c>
@@ -1850,7 +1936,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>0</v>
       </c>
@@ -1858,7 +1944,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>0</v>
       </c>
@@ -1866,7 +1952,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>0</v>
       </c>
@@ -1874,7 +1960,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>0</v>
       </c>
@@ -1882,20 +1968,28 @@
         <v>4</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>0</v>
       </c>
       <c r="B123">
         <v>0</v>
       </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D123">
+        <f t="shared" si="3"/>
+        <v>6.9245099999999992E-3</v>
+      </c>
+      <c r="E123">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>1.5622377E-2</v>
       </c>
@@ -1903,7 +1997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>0</v>
       </c>
@@ -1911,7 +2005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>0</v>
       </c>
@@ -1919,7 +2013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>1.5621901000000001E-2</v>
       </c>
@@ -1927,7 +2021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>0</v>
       </c>
@@ -1935,7 +2029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>0</v>
       </c>
@@ -1943,7 +2037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>1.5621184999999999E-2</v>
       </c>
@@ -1951,7 +2045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>1.5622139E-2</v>
       </c>
@@ -1959,7 +2053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>6.7574979999999998E-3</v>
       </c>
@@ -1967,20 +2061,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>0</v>
       </c>
       <c r="B134">
         <v>0</v>
       </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D134">
+        <f t="shared" si="3"/>
+        <v>7.0466042000000007E-3</v>
+      </c>
+      <c r="E134">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>0</v>
       </c>
@@ -1988,7 +2090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>1.5621901000000001E-2</v>
       </c>
@@ -1996,7 +2098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>0</v>
       </c>
@@ -2004,7 +2106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>3.9894580000000004E-3</v>
       </c>
@@ -2012,7 +2114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>1.5620708000000001E-2</v>
       </c>
@@ -2020,7 +2122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>1.5621424E-2</v>
       </c>
@@ -2028,7 +2130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>1.5622139E-2</v>
       </c>
@@ -2036,7 +2138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>0</v>
       </c>
@@ -2044,7 +2146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>3.9904119999999996E-3</v>
       </c>
@@ -2052,20 +2154,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>0</v>
       </c>
       <c r="B145">
         <v>0</v>
       </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D145">
+        <f t="shared" si="3"/>
+        <v>6.2500476999999997E-3</v>
+      </c>
+      <c r="E145">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>0</v>
       </c>
@@ -2073,7 +2183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>1.5621184999999999E-2</v>
       </c>
@@ -2081,7 +2191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>0</v>
       </c>
@@ -2089,7 +2199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>0</v>
       </c>
@@ -2097,7 +2207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>1.5621424E-2</v>
       </c>
@@ -2105,7 +2215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>0</v>
       </c>
@@ -2113,7 +2223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>1.5621662E-2</v>
       </c>
@@ -2121,7 +2231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>0</v>
       </c>
@@ -2129,7 +2239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>1.5636206E-2</v>
       </c>
@@ -2137,20 +2247,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>0</v>
       </c>
       <c r="B156">
         <v>0</v>
       </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D156">
+        <f t="shared" si="3"/>
+        <v>9.9635099999999997E-5</v>
+      </c>
+      <c r="E156">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>0</v>
       </c>
@@ -2158,7 +2276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>0</v>
       </c>
@@ -2166,7 +2284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>0</v>
       </c>
@@ -2174,7 +2292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>9.9635099999999992E-4</v>
       </c>
@@ -2182,7 +2300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>0</v>
       </c>
@@ -2190,7 +2308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>0</v>
       </c>
@@ -2198,7 +2316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>0</v>
       </c>
@@ -2206,7 +2324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>0</v>
       </c>
@@ -2214,7 +2332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>0</v>
       </c>
@@ -2222,20 +2340,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>0</v>
       </c>
       <c r="B167">
         <v>0</v>
       </c>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D167">
+        <f t="shared" ref="D164:D227" si="5">AVERAGE(A167:A176)</f>
+        <v>1.9953249999999999E-4</v>
+      </c>
+      <c r="E167">
+        <f t="shared" ref="E164:E227" si="6">AVERAGE(B167:B176)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>0</v>
       </c>
@@ -2243,7 +2369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>0</v>
       </c>
@@ -2251,7 +2377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>0</v>
       </c>
@@ -2259,7 +2385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>0</v>
       </c>
@@ -2267,7 +2393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>0</v>
       </c>
@@ -2275,7 +2401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>0</v>
       </c>
@@ -2283,7 +2409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>9.9754300000000004E-4</v>
       </c>
@@ -2291,7 +2417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>9.9778200000000001E-4</v>
       </c>
@@ -2299,7 +2425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>0</v>
       </c>
@@ -2307,20 +2433,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>0</v>
       </c>
       <c r="B178">
         <v>1</v>
       </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D178">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E178">
+        <f t="shared" si="6"/>
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>0</v>
       </c>
@@ -2328,7 +2462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>0</v>
       </c>
@@ -2336,7 +2470,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>0</v>
       </c>
@@ -2344,7 +2478,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>0</v>
       </c>
@@ -2352,7 +2486,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>0</v>
       </c>
@@ -2360,7 +2494,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>0</v>
       </c>
@@ -2368,7 +2502,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>0</v>
       </c>
@@ -2376,7 +2510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>0</v>
       </c>
@@ -2384,7 +2518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>0</v>
       </c>
@@ -2392,20 +2526,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>0</v>
       </c>
       <c r="B189">
         <v>0</v>
       </c>
-    </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D189">
+        <f t="shared" si="5"/>
+        <v>1.5622854E-3</v>
+      </c>
+      <c r="E189">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>0</v>
       </c>
@@ -2413,7 +2555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>1.5622854E-2</v>
       </c>
@@ -2421,7 +2563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>0</v>
       </c>
@@ -2429,7 +2571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>0</v>
       </c>
@@ -2437,7 +2579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>0</v>
       </c>
@@ -2445,7 +2587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>0</v>
       </c>
@@ -2453,7 +2595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>0</v>
       </c>
@@ -2461,7 +2603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>0</v>
       </c>
@@ -2469,7 +2611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>0</v>
       </c>
@@ -2477,20 +2619,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D199">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E199">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>0</v>
       </c>
       <c r="B200">
         <v>1</v>
       </c>
-    </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D200">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E200">
+        <f t="shared" si="6"/>
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>0</v>
       </c>
@@ -2498,7 +2656,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>0</v>
       </c>
@@ -2506,7 +2664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>0</v>
       </c>
@@ -2514,7 +2672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>0</v>
       </c>
@@ -2522,7 +2680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>0</v>
       </c>
@@ -2530,7 +2688,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>0</v>
       </c>
@@ -2538,7 +2696,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>0</v>
       </c>
@@ -2546,7 +2704,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>0</v>
       </c>
@@ -2554,7 +2712,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>0</v>
       </c>
@@ -2562,20 +2720,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>0</v>
       </c>
       <c r="B211">
         <v>31</v>
       </c>
-    </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D211">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E211">
+        <f t="shared" si="6"/>
+        <v>17.899999999999999</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>0</v>
       </c>
@@ -2583,7 +2749,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>0</v>
       </c>
@@ -2591,7 +2757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>0</v>
       </c>
@@ -2599,7 +2765,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>0</v>
       </c>
@@ -2607,7 +2773,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>0</v>
       </c>
@@ -2615,7 +2781,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>0</v>
       </c>
@@ -2623,7 +2789,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>0</v>
       </c>
@@ -2631,7 +2797,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>0</v>
       </c>
@@ -2639,7 +2805,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>0</v>
       </c>
@@ -2647,20 +2813,28 @@
         <v>35</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>0</v>
       </c>
       <c r="B222">
         <v>0</v>
       </c>
-    </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D222">
+        <f t="shared" si="5"/>
+        <v>1.6617775000000001E-3</v>
+      </c>
+      <c r="E222">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>0</v>
       </c>
@@ -2668,7 +2842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>0</v>
       </c>
@@ -2676,7 +2850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>9.9682799999999995E-4</v>
       </c>
@@ -2684,7 +2858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>0</v>
       </c>
@@ -2692,7 +2866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>0</v>
       </c>
@@ -2700,7 +2874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>0</v>
       </c>
@@ -2708,7 +2882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>1.5620947E-2</v>
       </c>
@@ -2716,7 +2890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>0</v>
       </c>
@@ -2724,7 +2898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>0</v>
       </c>
@@ -2732,20 +2906,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>0</v>
       </c>
       <c r="B233">
         <v>0</v>
       </c>
-    </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D233">
+        <f t="shared" ref="D228:D291" si="7">AVERAGE(A233:A242)</f>
+        <v>2.9909610000000003E-4</v>
+      </c>
+      <c r="E233">
+        <f t="shared" ref="E228:E291" si="8">AVERAGE(B233:B242)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>0</v>
       </c>
@@ -2753,7 +2935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>0</v>
       </c>
@@ -2761,7 +2943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>9.9563600000000005E-4</v>
       </c>
@@ -2769,7 +2951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>0</v>
       </c>
@@ -2777,7 +2959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>9.9754300000000004E-4</v>
       </c>
@@ -2785,7 +2967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>0</v>
       </c>
@@ -2793,7 +2975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>9.9778200000000001E-4</v>
       </c>
@@ -2801,7 +2983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A241">
         <v>0</v>
       </c>
@@ -2809,7 +2991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A242">
         <v>0</v>
       </c>
@@ -2817,20 +2999,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A244">
         <v>0</v>
       </c>
       <c r="B244">
         <v>1</v>
       </c>
-    </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D244">
+        <f t="shared" si="7"/>
+        <v>1.9950870000000001E-4</v>
+      </c>
+      <c r="E244">
+        <f t="shared" si="8"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A245">
         <v>0</v>
       </c>
@@ -2838,7 +3028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A246">
         <v>0</v>
       </c>
@@ -2846,7 +3036,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A247">
         <v>0</v>
       </c>
@@ -2854,7 +3044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A248">
         <v>1.995087E-3</v>
       </c>
@@ -2862,7 +3052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A249">
         <v>0</v>
       </c>
@@ -2870,7 +3060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A250">
         <v>0</v>
       </c>
@@ -2878,7 +3068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A251">
         <v>0</v>
       </c>
@@ -2886,7 +3076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A252">
         <v>0</v>
       </c>
@@ -2894,7 +3084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A253">
         <v>0</v>
       </c>
@@ -2902,20 +3092,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A255">
         <v>0</v>
       </c>
       <c r="B255">
         <v>0</v>
       </c>
-    </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D255">
+        <f t="shared" si="7"/>
+        <v>1.6620636000000001E-3</v>
+      </c>
+      <c r="E255">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A256">
         <v>1.5622616000000001E-2</v>
       </c>
@@ -2923,7 +3121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A257">
         <v>0</v>
       </c>
@@ -2931,7 +3129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A258">
         <v>0</v>
       </c>
@@ -2939,7 +3137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A259">
         <v>0</v>
       </c>
@@ -2947,7 +3145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A260">
         <v>0</v>
       </c>
@@ -2955,7 +3153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A261">
         <v>9.9802000000000007E-4</v>
       </c>
@@ -2963,7 +3161,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A262">
         <v>0</v>
       </c>
@@ -2971,7 +3169,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A263">
         <v>0</v>
       </c>
@@ -2979,7 +3177,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A264">
         <v>0</v>
       </c>
@@ -2987,20 +3185,36 @@
         <v>1</v>
       </c>
     </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D265">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E265">
+        <f t="shared" si="8"/>
+        <v>0.1111111111111111</v>
+      </c>
+    </row>
+    <row r="266" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A266">
         <v>0</v>
       </c>
       <c r="B266">
         <v>1</v>
       </c>
-    </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D266">
+        <f>AVERAGE(A266:A275)</f>
+        <v>0</v>
+      </c>
+      <c r="E266">
+        <f t="shared" si="8"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="267" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A267">
         <v>0</v>
       </c>
@@ -3008,7 +3222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A268">
         <v>0</v>
       </c>
@@ -3016,7 +3230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A269">
         <v>0</v>
       </c>
@@ -3024,7 +3238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A270">
         <v>0</v>
       </c>
@@ -3032,7 +3246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A271">
         <v>0</v>
       </c>
@@ -3040,7 +3254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A272">
         <v>0</v>
       </c>
@@ -3048,7 +3262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A273">
         <v>0</v>
       </c>
@@ -3056,7 +3270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A274">
         <v>0</v>
       </c>
@@ -3064,7 +3278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A275">
         <v>0</v>
       </c>
@@ -3072,28 +3286,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A276">
-        <v>0</v>
-      </c>
-      <c r="B276">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A278">
         <v>9.9730499999999998E-4</v>
       </c>
       <c r="B278">
         <v>27</v>
       </c>
-    </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D278">
+        <f>AVERAGE(A278:A287)</f>
+        <v>9.9730500000000003E-5</v>
+      </c>
+      <c r="E278">
+        <f t="shared" si="8"/>
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="279" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A279">
         <v>0</v>
       </c>
@@ -3101,7 +3315,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A280">
         <v>0</v>
       </c>
@@ -3109,7 +3323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A281">
         <v>0</v>
       </c>
@@ -3117,7 +3331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A282">
         <v>0</v>
       </c>
@@ -3125,7 +3339,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A283">
         <v>0</v>
       </c>
@@ -3133,7 +3347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A284">
         <v>0</v>
       </c>
@@ -3141,7 +3355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A285">
         <v>0</v>
       </c>
@@ -3149,7 +3363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A286">
         <v>0</v>
       </c>
@@ -3157,7 +3371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A287">
         <v>0</v>
       </c>
@@ -3165,20 +3379,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A289">
         <v>0</v>
       </c>
       <c r="B289">
         <v>0</v>
       </c>
-    </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D289">
+        <f>AVERAGE(A289:A298)</f>
+        <v>0</v>
+      </c>
+      <c r="E289">
+        <f>AVERAGE(B289:B298)</f>
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="290" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A290">
         <v>0</v>
       </c>
@@ -3186,7 +3408,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A291">
         <v>0</v>
       </c>
@@ -3194,7 +3416,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A292">
         <v>0</v>
       </c>
@@ -3202,7 +3424,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A293">
         <v>0</v>
       </c>
@@ -3210,7 +3432,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A294">
         <v>0</v>
       </c>
@@ -3218,7 +3440,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A295">
         <v>0</v>
       </c>
@@ -3226,7 +3448,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A296">
         <v>0</v>
       </c>
@@ -3234,12 +3456,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A297">
         <v>0</v>
       </c>
       <c r="B297">
         <v>8</v>
+      </c>
+    </row>
+    <row r="298" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A298">
+        <v>0</v>
+      </c>
+      <c r="B298">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>